<commit_message>
atualizando documentacao e atributos do BD
</commit_message>
<xml_diff>
--- a/Documentação Técnica - BuscaFarma.xlsx
+++ b/Documentação Técnica - BuscaFarma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbbcd6cf5880efa7/Documentos/Mestrado/Projeto BD_EngSoft/PPGTI_2024-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{1CEC9063-15EE-4A30-9E9D-91E2DE7AC9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBB87FC0-286D-4F46-AE99-816DDB13C0EC}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{1CEC9063-15EE-4A30-9E9D-91E2DE7AC9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50459793-0F27-49E6-BE46-9C18D826ADED}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t xml:space="preserve">Responsáveis: </t>
   </si>
@@ -65,9 +65,6 @@
     <t>Fato_Csmo_Invs_Diva</t>
   </si>
   <si>
-    <t>Origem</t>
-  </si>
-  <si>
     <t>SPCBI.FT_CONSULENTE_MENSAL</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Nome Lógico do Campo</t>
   </si>
   <si>
-    <t>Descrição do Campo</t>
-  </si>
-  <si>
     <t>Definição Funcional</t>
   </si>
   <si>
@@ -110,72 +104,9 @@
     <t>Tamanho</t>
   </si>
   <si>
-    <t>Nome Arquivo / Schema</t>
-  </si>
-  <si>
-    <t>Planilha / Tabela</t>
-  </si>
-  <si>
     <t>Campo</t>
   </si>
   <si>
-    <t>SK que identifica a Data</t>
-  </si>
-  <si>
-    <t>NUMBER</t>
-  </si>
-  <si>
-    <t>SPCBI</t>
-  </si>
-  <si>
-    <t>DM_DATA</t>
-  </si>
-  <si>
-    <t>ID_DM_DATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data de Inclusao </t>
-  </si>
-  <si>
-    <t>Data de inclusão do registro nas bases</t>
-  </si>
-  <si>
-    <t>SPCBI/FITSIS</t>
-  </si>
-  <si>
-    <t>SPCBI.FT_SPC_CHQ_OPERACAO_INCL_MES - SPCBI.FT_CONSULENTE_MENSAL/FITSIS.EA10_CONSULTA_REAL_SRS_TOTAL - FITSIS.BI_ANOTACAO</t>
-  </si>
-  <si>
-    <t>DT_REF - DT_INCLUSAO / DAT_CONSULTA - DAT_INCLUSAO</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>Surrogate key Dimensão Entidade</t>
-  </si>
-  <si>
-    <t>SK que identifica da Entidade</t>
-  </si>
-  <si>
-    <t>DM_ENTIDADE</t>
-  </si>
-  <si>
-    <t>ID_DM_ENTIDADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surrogate key Dimensão Cidade </t>
-  </si>
-  <si>
-    <t>SK que identifica a Cidade da Entidade</t>
-  </si>
-  <si>
-    <t>DM_CIDADE</t>
-  </si>
-  <si>
-    <t>ID_DM_CIDADE</t>
-  </si>
-  <si>
     <t>ID_DM_ASSOCIADO</t>
   </si>
   <si>
@@ -269,7 +200,58 @@
     <t>String</t>
   </si>
   <si>
-    <t>nome jurídico da farmacia</t>
+    <t>cnpj</t>
+  </si>
+  <si>
+    <t>situacao</t>
+  </si>
+  <si>
+    <t>cnpj da farmácia</t>
+  </si>
+  <si>
+    <t>nome jurídico da farmácia</t>
+  </si>
+  <si>
+    <t>rua</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>bairro</t>
+  </si>
+  <si>
+    <t>municipio</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>nome fantasia da farmácia</t>
+  </si>
+  <si>
+    <t>coordenadas geográficas da farmácia</t>
+  </si>
+  <si>
+    <t>situação cadastral do cnpj da farmácia</t>
+  </si>
+  <si>
+    <t>rua da farmácia</t>
+  </si>
+  <si>
+    <t>numero do endereço da farmácia</t>
+  </si>
+  <si>
+    <t>bairro da farmácia</t>
+  </si>
+  <si>
+    <t>cidade da farmácia</t>
+  </si>
+  <si>
+    <t>estado da farmácia</t>
+  </si>
+  <si>
+    <t>endereço completo da farmácia, objeto que contem rua + numero + bairro</t>
   </si>
 </sst>
 </file>
@@ -277,9 +259,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,8 +307,27 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,18 +354,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -382,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -484,19 +473,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -722,124 +698,112 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Moeda 2" xfId="2" xr:uid="{1F098F58-AFD7-4D6C-BFFB-E8DC77DE9DC5}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -999,6 +963,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1314,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1402,428 +1370,429 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="90" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="37">
+        <v>1</v>
+      </c>
+      <c r="B20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="3" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="C20" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="22" t="s">
+      <c r="D20" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="24" t="s">
+      <c r="F20" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="37">
+        <v>2</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37">
+        <v>3</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="37">
+        <v>4</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="28"/>
-    </row>
-    <row r="5" spans="1:12" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="E23" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="27" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="37">
+        <v>5</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="E24" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="24" t="s">
+      <c r="F24" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="40">
+        <v>6</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="28"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="E25" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="24" t="s">
+      <c r="F25" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="42">
+        <v>7</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="28"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="24" t="s">
+      <c r="D26" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="F26" s="41" t="s">
         <v>41</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="28"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-    </row>
-    <row r="11" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="45"/>
-    </row>
-    <row r="14" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="46">
-        <v>1</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46">
-        <v>2</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="46">
-        <v>3</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="46">
-        <v>4</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="46">
-        <v>5</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="49">
-        <v>6</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="52">
-        <v>7</v>
-      </c>
-      <c r="B20" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="53" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1842,7 +1811,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -1850,7 +1819,7 @@
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
atualizando json removendo espacos e att arquivo pptx
</commit_message>
<xml_diff>
--- a/Documentação Técnica - BuscaFarma.xlsx
+++ b/Documentação Técnica - BuscaFarma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbbcd6cf5880efa7/Documentos/Mestrado/Projeto BD_EngSoft/PPGTI_2024-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{1CEC9063-15EE-4A30-9E9D-91E2DE7AC9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50459793-0F27-49E6-BE46-9C18D826ADED}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{1CEC9063-15EE-4A30-9E9D-91E2DE7AC9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{938B1A5C-E014-4908-833B-441504AD6497}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -699,9 +699,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -742,25 +742,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -797,6 +781,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1372,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1400,7 +1399,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="39" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1420,7 +1419,7 @@
       <c r="E3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -1490,7 +1489,7 @@
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1607,184 +1606,184 @@
       <c r="F15" s="21"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="26" t="s">
+      <c r="E18" s="29"/>
+      <c r="F18" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="30" t="s">
+      <c r="A19" s="42"/>
+      <c r="B19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="45"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="37">
+      <c r="A20" s="31">
         <v>1</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="37">
+      <c r="A21" s="31">
         <v>2</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="37">
+      <c r="A22" s="31">
         <v>3</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="37">
+      <c r="A23" s="31">
         <v>4</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37">
+      <c r="A24" s="31">
         <v>5</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="40">
+      <c r="A25" s="34">
         <v>6</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="44" t="s">
+      <c r="F25" s="38" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="42">
+      <c r="A26" s="36">
         <v>7</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="35" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>